<commit_message>
finished all of the code for checkpoint 1
</commit_message>
<xml_diff>
--- a/data/clean data/summary stats_discount_0.1.xlsx
+++ b/data/clean data/summary stats_discount_0.1.xlsx
@@ -645,16 +645,16 @@
         <v>82</v>
       </c>
       <c r="W2">
-        <v>1119038.132242292</v>
+        <v>1186143.786628215</v>
       </c>
       <c r="X2">
-        <v>354191.2696469671</v>
+        <v>372026.4514100465</v>
       </c>
       <c r="Y2">
-        <v>215014.3491087809</v>
+        <v>224237.1260771329</v>
       </c>
       <c r="Z2">
-        <v>1916923.803584612</v>
+        <v>2022870.84887259</v>
       </c>
       <c r="AA2" t="s">
         <v>8</v>
@@ -665,64 +665,64 @@
         <v>31</v>
       </c>
       <c r="C3">
-        <v>404.4853140588061</v>
+        <v>422.7975147288581</v>
       </c>
       <c r="D3">
-        <v>814.5227973483621</v>
+        <v>860.1184454417242</v>
       </c>
       <c r="E3">
-        <v>1148.844232521158</v>
+        <v>1220.109252469695</v>
       </c>
       <c r="F3">
-        <v>1395.984945903953</v>
+        <v>1483.808806566078</v>
       </c>
       <c r="G3">
-        <v>1573.160414338761</v>
+        <v>1669.107300248349</v>
       </c>
       <c r="H3">
-        <v>1653.009209767582</v>
+        <v>1763.020366268689</v>
       </c>
       <c r="I3">
-        <v>1674.635175609382</v>
+        <v>1777.283032786893</v>
       </c>
       <c r="J3">
-        <v>1651.959350482833</v>
+        <v>1747.364755055248</v>
       </c>
       <c r="K3">
-        <v>1588.059541270139</v>
+        <v>1674.941448011221</v>
       </c>
       <c r="L3">
-        <v>1500.059922447675</v>
+        <v>1581.548387486778</v>
       </c>
       <c r="M3">
-        <v>1391.965320406664</v>
+        <v>1464.01984374749</v>
       </c>
       <c r="N3">
-        <v>1266.079325544549</v>
+        <v>1326.697612819901</v>
       </c>
       <c r="O3">
-        <v>1109.947584335671</v>
+        <v>1167.010749922465</v>
       </c>
       <c r="P3">
-        <v>932.7065944307586</v>
+        <v>976.5737907812552</v>
       </c>
       <c r="Q3">
-        <v>731.0391458945666</v>
+        <v>764.273327304071</v>
       </c>
       <c r="R3">
-        <v>529.4949179619565</v>
+        <v>555.4291892810566</v>
       </c>
       <c r="S3">
-        <v>386.3453836735512</v>
+        <v>403.3504963809903</v>
       </c>
       <c r="T3">
-        <v>300.2048831309363</v>
+        <v>311.182687875175</v>
       </c>
       <c r="U3">
-        <v>233.1420584386646</v>
+        <v>238.8718159538598</v>
       </c>
       <c r="V3">
-        <v>182.1842354415789</v>
+        <v>190.3445911086999</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -730,64 +730,64 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>613.9813041548377</v>
+        <v>607.1538275467569</v>
       </c>
       <c r="D4">
-        <v>1037.258804886535</v>
+        <v>1014.593899524785</v>
       </c>
       <c r="E4">
-        <v>1321.829081629988</v>
+        <v>1280.71948706914</v>
       </c>
       <c r="F4">
-        <v>1533.572677058429</v>
+        <v>1475.422760399498</v>
       </c>
       <c r="G4">
-        <v>1751.379780186113</v>
+        <v>1688.626750233924</v>
       </c>
       <c r="H4">
-        <v>1894.873851139746</v>
+        <v>1831.858104829752</v>
       </c>
       <c r="I4">
-        <v>1925.528681406684</v>
+        <v>1864.83812985111</v>
       </c>
       <c r="J4">
-        <v>1893.827777033972</v>
+        <v>1831.001080697439</v>
       </c>
       <c r="K4">
-        <v>1840.646824529918</v>
+        <v>1779.51987012943</v>
       </c>
       <c r="L4">
-        <v>1777.037860881826</v>
+        <v>1722.104798449825</v>
       </c>
       <c r="M4">
-        <v>1681.284357771098</v>
+        <v>1631.096637514034</v>
       </c>
       <c r="N4">
-        <v>1566.499587800422</v>
+        <v>1523.992494553101</v>
       </c>
       <c r="O4">
-        <v>1438.590047186498</v>
+        <v>1406.252271110642</v>
       </c>
       <c r="P4">
-        <v>1279.505779214467</v>
+        <v>1258.364105727699</v>
       </c>
       <c r="Q4">
-        <v>1010.875257060343</v>
+        <v>997.4637424948185</v>
       </c>
       <c r="R4">
-        <v>738.6940750333899</v>
+        <v>732.0866896440704</v>
       </c>
       <c r="S4">
-        <v>622.6485131703918</v>
+        <v>617.8398595851485</v>
       </c>
       <c r="T4">
-        <v>554.4347233996052</v>
+        <v>549.6214528291041</v>
       </c>
       <c r="U4">
-        <v>496.1149228905821</v>
+        <v>487.5190906994106</v>
       </c>
       <c r="V4">
-        <v>450.9409921331971</v>
+        <v>449.9765983518436</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -798,43 +798,43 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.516500735759003</v>
+        <v>27.59809698814373</v>
       </c>
       <c r="E5">
-        <v>1.658009997523121</v>
+        <v>38.44540183260668</v>
       </c>
       <c r="F5">
-        <v>2.096724917376689</v>
+        <v>115.8589374133198</v>
       </c>
       <c r="G5">
-        <v>2.881754965632149</v>
+        <v>170.7581151357477</v>
       </c>
       <c r="H5">
-        <v>2.867229007583833</v>
+        <v>171.9046939261023</v>
       </c>
       <c r="I5">
-        <v>1.433512597090133</v>
+        <v>120.4893558152518</v>
       </c>
       <c r="J5">
-        <v>3.626687400423816</v>
+        <v>52.2628412471144</v>
       </c>
       <c r="K5">
-        <v>3.379895878061367</v>
+        <v>28.31234334638594</v>
       </c>
       <c r="L5">
-        <v>4.000447390135247</v>
+        <v>17.83900293929106</v>
       </c>
       <c r="M5">
-        <v>4.801914332256297</v>
+        <v>12.5939441407318</v>
       </c>
       <c r="N5">
-        <v>4.155567300485678</v>
+        <v>9.480095953501099</v>
       </c>
       <c r="O5">
-        <v>3.626771209981159</v>
+        <v>7.319607890530854</v>
       </c>
       <c r="P5">
-        <v>3.192682994078432</v>
+        <v>5.738900787893129</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -860,64 +860,64 @@
         <v>34</v>
       </c>
       <c r="C6">
-        <v>84.57789407100728</v>
+        <v>109.9408772822171</v>
       </c>
       <c r="D6">
-        <v>192.5358607486798</v>
+        <v>247.201848997351</v>
       </c>
       <c r="E6">
-        <v>302.1331519327155</v>
+        <v>400.3155291032056</v>
       </c>
       <c r="F6">
-        <v>400.252907063491</v>
+        <v>524.1283829616048</v>
       </c>
       <c r="G6">
-        <v>403.8539701587715</v>
+        <v>603.6309946505204</v>
       </c>
       <c r="H6">
-        <v>491.4551152975694</v>
+        <v>660.4634324785502</v>
       </c>
       <c r="I6">
-        <v>477.9751026096095</v>
+        <v>647.0311379462704</v>
       </c>
       <c r="J6">
-        <v>418.2958595577335</v>
+        <v>606.3379864060973</v>
       </c>
       <c r="K6">
-        <v>434.3289564539924</v>
+        <v>587.7412794786894</v>
       </c>
       <c r="L6">
-        <v>408.5167248935237</v>
+        <v>545.6439474101549</v>
       </c>
       <c r="M6">
-        <v>343.6917979212957</v>
+        <v>473.6408332167913</v>
       </c>
       <c r="N6">
-        <v>289.0198504745238</v>
+        <v>398.377563382784</v>
       </c>
       <c r="O6">
-        <v>245.5303046380066</v>
+        <v>323.1524955644614</v>
       </c>
       <c r="P6">
-        <v>158.4793813657931</v>
+        <v>236.6695116150312</v>
       </c>
       <c r="Q6">
-        <v>105.5800438084709</v>
+        <v>162.001149725539</v>
       </c>
       <c r="R6">
-        <v>79.22540077233663</v>
+        <v>101.5630297819396</v>
       </c>
       <c r="S6">
-        <v>55.90322404529971</v>
+        <v>72.62141703012223</v>
       </c>
       <c r="T6">
-        <v>35.50917325488845</v>
+        <v>51.08671692159405</v>
       </c>
       <c r="U6">
-        <v>24.24816206591179</v>
+        <v>33.89716282207043</v>
       </c>
       <c r="V6">
-        <v>18.17675242991613</v>
+        <v>24.7721153895701</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -925,64 +925,64 @@
         <v>35</v>
       </c>
       <c r="C7">
-        <v>222.6656032611668</v>
+        <v>225.402728512642</v>
       </c>
       <c r="D7">
-        <v>453.1841827160412</v>
+        <v>507.2968188800573</v>
       </c>
       <c r="E7">
-        <v>725.5171019169967</v>
+        <v>802.5439090604442</v>
       </c>
       <c r="F7">
-        <v>862.6525554796438</v>
+        <v>963.9902652402343</v>
       </c>
       <c r="G7">
-        <v>928.4130093819454</v>
+        <v>1062.447764450607</v>
       </c>
       <c r="H7">
-        <v>941.534173967557</v>
+        <v>1086.75968002611</v>
       </c>
       <c r="I7">
-        <v>981.439161022952</v>
+        <v>1123.365802645769</v>
       </c>
       <c r="J7">
-        <v>1052.948627526411</v>
+        <v>1142.242603046327</v>
       </c>
       <c r="K7">
-        <v>933.9931424207977</v>
+        <v>1059.328418354073</v>
       </c>
       <c r="L7">
-        <v>793.7085861312282</v>
+        <v>894.1415514000266</v>
       </c>
       <c r="M7">
-        <v>752.346726463161</v>
+        <v>827.4151382073626</v>
       </c>
       <c r="N7">
-        <v>684.4922711078118</v>
+        <v>764.82863821909</v>
       </c>
       <c r="O7">
-        <v>556.6441188475026</v>
+        <v>671.6956011869682</v>
       </c>
       <c r="P7">
-        <v>449.2197067704695</v>
+        <v>511.7619998472665</v>
       </c>
       <c r="Q7">
-        <v>301.6841884090871</v>
+        <v>346.1648883240642</v>
       </c>
       <c r="R7">
-        <v>249.6551228474298</v>
+        <v>277.8099920850848</v>
       </c>
       <c r="S7">
-        <v>166.3950141191223</v>
+        <v>183.1426767645817</v>
       </c>
       <c r="T7">
-        <v>113.064581072388</v>
+        <v>135.8035516160135</v>
       </c>
       <c r="U7">
-        <v>90.28797141493035</v>
+        <v>96.02377550354682</v>
       </c>
       <c r="V7">
-        <v>66.71987443632756</v>
+        <v>81.61662236086295</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -990,64 +990,64 @@
         <v>36</v>
       </c>
       <c r="C8">
-        <v>474.8655701611422</v>
+        <v>510.2372426783423</v>
       </c>
       <c r="D8">
-        <v>909.7437632919637</v>
+        <v>925.8149861003142</v>
       </c>
       <c r="E8">
-        <v>1593.438316747206</v>
+        <v>1612.979072293257</v>
       </c>
       <c r="F8">
-        <v>1872.266091689984</v>
+        <v>1820.41913557115</v>
       </c>
       <c r="G8">
-        <v>1965.748903261281</v>
+        <v>1965.748879405097</v>
       </c>
       <c r="H8">
-        <v>1968.933528431255</v>
+        <v>1966.521126356225</v>
       </c>
       <c r="I8">
-        <v>2046.823984628528</v>
+        <v>2046.82448557963</v>
       </c>
       <c r="J8">
-        <v>2130.169353291804</v>
+        <v>2031.320756238682</v>
       </c>
       <c r="K8">
-        <v>2098.030924555171</v>
+        <v>2022.338712159301</v>
       </c>
       <c r="L8">
-        <v>2114.150155789438</v>
+        <v>2114.149107901399</v>
       </c>
       <c r="M8">
-        <v>2025.815439258065</v>
+        <v>2025.816119401169</v>
       </c>
       <c r="N8">
-        <v>1841.499809905733</v>
+        <v>1685.151724157374</v>
       </c>
       <c r="O8">
-        <v>1496.101374676056</v>
+        <v>1496.101589999149</v>
       </c>
       <c r="P8">
-        <v>1236.182473261289</v>
+        <v>1213.252514625557</v>
       </c>
       <c r="Q8">
-        <v>940.3119112288497</v>
+        <v>931.8583249161615</v>
       </c>
       <c r="R8">
-        <v>608.5091004849947</v>
+        <v>631.4678460176002</v>
       </c>
       <c r="S8">
-        <v>376.3867914776888</v>
+        <v>441.3321434326957</v>
       </c>
       <c r="T8">
-        <v>270.6237826805323</v>
+        <v>299.9648726993082</v>
       </c>
       <c r="U8">
-        <v>196.8842792597378</v>
+        <v>208.084454744136</v>
       </c>
       <c r="V8">
-        <v>145.0912374288697</v>
+        <v>161.5225907913373</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1055,64 +1055,64 @@
         <v>37</v>
       </c>
       <c r="C9">
-        <v>3858.281431215651</v>
+        <v>3858.284906931097</v>
       </c>
       <c r="D9">
-        <v>5006.318502195393</v>
+        <v>5006.321567132402</v>
       </c>
       <c r="E9">
         <v>6620.195513697532</v>
       </c>
       <c r="F9">
-        <v>6781.409826678473</v>
+        <v>6781.410831816548</v>
       </c>
       <c r="G9">
-        <v>8968.133032954333</v>
+        <v>8968.132758815722</v>
       </c>
       <c r="H9">
-        <v>10248.82631385416</v>
+        <v>10248.82600825178</v>
       </c>
       <c r="I9">
-        <v>10443.23211779421</v>
+        <v>10443.2322406751</v>
       </c>
       <c r="J9">
-        <v>10183.05212786518</v>
+        <v>10183.05233112912</v>
       </c>
       <c r="K9">
-        <v>10043.91290342726</v>
+        <v>10043.91171350932</v>
       </c>
       <c r="L9">
-        <v>9954.173837864944</v>
+        <v>9954.173921107971</v>
       </c>
       <c r="M9">
-        <v>9621.855013641352</v>
+        <v>9621.855311878877</v>
       </c>
       <c r="N9">
-        <v>9133.675257549938</v>
+        <v>9133.674309114305</v>
       </c>
       <c r="O9">
-        <v>8570.98680761433</v>
+        <v>8570.985889542053</v>
       </c>
       <c r="P9">
-        <v>7636.955613259365</v>
+        <v>7636.954855722198</v>
       </c>
       <c r="Q9">
-        <v>5368.939801829926</v>
+        <v>5368.939138667408</v>
       </c>
       <c r="R9">
-        <v>4147.629781810328</v>
+        <v>4147.629694390414</v>
       </c>
       <c r="S9">
-        <v>4406.245289672</v>
+        <v>4406.245349718633</v>
       </c>
       <c r="T9">
-        <v>4131.941208744907</v>
+        <v>4131.941378170714</v>
       </c>
       <c r="U9">
-        <v>3849.479355905137</v>
+        <v>3849.479391138518</v>
       </c>
       <c r="V9">
-        <v>3599.268303743567</v>
+        <v>3599.26841923676</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1120,64 +1120,64 @@
         <v>38</v>
       </c>
       <c r="C10">
-        <v>38021.61952152776</v>
+        <v>39742.96638451266</v>
       </c>
       <c r="D10">
-        <v>76565.14295074604</v>
+        <v>80851.13387152206</v>
       </c>
       <c r="E10">
-        <v>107991.3578569889</v>
+        <v>114690.2697321513</v>
       </c>
       <c r="F10">
-        <v>131222.5849149716</v>
+        <v>139478.0278172114</v>
       </c>
       <c r="G10">
-        <v>147877.0789478435</v>
+        <v>156896.0862233449</v>
       </c>
       <c r="H10">
-        <v>155382.8657181527</v>
+        <v>165723.9144292568</v>
       </c>
       <c r="I10">
-        <v>157415.7065072819</v>
+        <v>167064.605081968</v>
       </c>
       <c r="J10">
-        <v>155284.1789453863</v>
+        <v>164252.2869751933</v>
       </c>
       <c r="K10">
-        <v>149277.596879393</v>
+        <v>157444.4961130548</v>
       </c>
       <c r="L10">
-        <v>141005.6327100815</v>
+        <v>148665.5484237571</v>
       </c>
       <c r="M10">
-        <v>130844.7401182264</v>
+        <v>137617.865312264</v>
       </c>
       <c r="N10">
-        <v>119011.4566011876</v>
+        <v>124709.5756050707</v>
       </c>
       <c r="O10">
-        <v>104335.0729275531</v>
+        <v>109699.0104927117</v>
       </c>
       <c r="P10">
-        <v>87674.41987649129</v>
+        <v>91797.93633343797</v>
       </c>
       <c r="Q10">
-        <v>67986.64056819469</v>
+        <v>71077.41943927859</v>
       </c>
       <c r="R10">
-        <v>49243.02737046196</v>
+        <v>51654.91460313827</v>
       </c>
       <c r="S10">
-        <v>35543.77529796673</v>
+        <v>37108.2456670511</v>
       </c>
       <c r="T10">
-        <v>27018.43948178425</v>
+        <v>28006.44190876575</v>
       </c>
       <c r="U10">
-        <v>20283.35908416383</v>
+        <v>20781.8479879858</v>
       </c>
       <c r="V10">
-        <v>14939.10730620947</v>
+        <v>15608.25647091339</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -1248,16 +1248,16 @@
         <v>54</v>
       </c>
       <c r="W11">
-        <v>653426.2561444546</v>
+        <v>712297.6156212939</v>
       </c>
       <c r="X11">
-        <v>183068.6972374878</v>
+        <v>200249.6629066761</v>
       </c>
       <c r="Y11">
-        <v>105550.0807256675</v>
+        <v>113453.206886898</v>
       </c>
       <c r="Z11">
-        <v>1061080.763483529</v>
+        <v>1156092.683510994</v>
       </c>
       <c r="AA11" t="s">
         <v>7</v>
@@ -1268,64 +1268,64 @@
         <v>31</v>
       </c>
       <c r="C12">
-        <v>386.1136269049228</v>
+        <v>410.9829406713303</v>
       </c>
       <c r="D12">
-        <v>744.7347172497382</v>
+        <v>805.4650771741366</v>
       </c>
       <c r="E12">
-        <v>1029.570073281459</v>
+        <v>1117.603592475667</v>
       </c>
       <c r="F12">
-        <v>1208.306019510807</v>
+        <v>1319.63266828842</v>
       </c>
       <c r="G12">
-        <v>1356.94993909797</v>
+        <v>1479.870143845559</v>
       </c>
       <c r="H12">
-        <v>1418.15054975764</v>
+        <v>1550.880843626675</v>
       </c>
       <c r="I12">
-        <v>1415.045642858194</v>
+        <v>1541.244144239174</v>
       </c>
       <c r="J12">
-        <v>1368.739906240504</v>
+        <v>1498.582150211546</v>
       </c>
       <c r="K12">
-        <v>1282.174777355865</v>
+        <v>1405.388683550207</v>
       </c>
       <c r="L12">
-        <v>1184.261776632004</v>
+        <v>1295.559143338067</v>
       </c>
       <c r="M12">
-        <v>1076.818354633346</v>
+        <v>1177.927078986875</v>
       </c>
       <c r="N12">
-        <v>958.2950923549812</v>
+        <v>1046.314080273425</v>
       </c>
       <c r="O12">
-        <v>825.3349473474187</v>
+        <v>904.659823656515</v>
       </c>
       <c r="P12">
-        <v>675.6714948667283</v>
+        <v>737.1314519138982</v>
       </c>
       <c r="Q12">
-        <v>527.6269883278626</v>
+        <v>574.0427256790742</v>
       </c>
       <c r="R12">
-        <v>380.099621873809</v>
+        <v>412.5049018680039</v>
       </c>
       <c r="S12">
-        <v>286.0058673966591</v>
+        <v>306.1248386000752</v>
       </c>
       <c r="T12">
-        <v>221.9440291522147</v>
+        <v>234.8648329681528</v>
       </c>
       <c r="U12">
-        <v>164.4361534107553</v>
+        <v>173.5482451123928</v>
       </c>
       <c r="V12">
-        <v>144.018552915049</v>
+        <v>151.1718178448053</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -1333,64 +1333,64 @@
         <v>32</v>
       </c>
       <c r="C13">
-        <v>703.6580724454953</v>
+        <v>698.6544960586658</v>
       </c>
       <c r="D13">
-        <v>1116.217658667673</v>
+        <v>1096.559026131998</v>
       </c>
       <c r="E13">
-        <v>1389.7029308292</v>
+        <v>1355.472038575006</v>
       </c>
       <c r="F13">
-        <v>1506.387781824983</v>
+        <v>1461.881409095709</v>
       </c>
       <c r="G13">
-        <v>1685.60253647086</v>
+        <v>1635.789161004483</v>
       </c>
       <c r="H13">
-        <v>1791.698926682969</v>
+        <v>1739.847768277564</v>
       </c>
       <c r="I13">
-        <v>1784.643622111867</v>
+        <v>1740.889784629405</v>
       </c>
       <c r="J13">
-        <v>1709.558161833719</v>
+        <v>1662.352736304708</v>
       </c>
       <c r="K13">
-        <v>1598.194938356492</v>
+        <v>1554.179239556446</v>
       </c>
       <c r="L13">
-        <v>1502.138835771782</v>
+        <v>1464.566980951382</v>
       </c>
       <c r="M13">
-        <v>1396.023292514612</v>
+        <v>1359.685905824596</v>
       </c>
       <c r="N13">
-        <v>1276.329255720576</v>
+        <v>1245.00769015443</v>
       </c>
       <c r="O13">
-        <v>1149.982913409994</v>
+        <v>1126.942239185938</v>
       </c>
       <c r="P13">
-        <v>1022.09074339027</v>
+        <v>1010.056433646611</v>
       </c>
       <c r="Q13">
-        <v>853.9099709106898</v>
+        <v>848.9414500358537</v>
       </c>
       <c r="R13">
-        <v>650.6425407139822</v>
+        <v>647.4784518341647</v>
       </c>
       <c r="S13">
-        <v>620.9720213052786</v>
+        <v>617.083282048952</v>
       </c>
       <c r="T13">
-        <v>570.1853540685989</v>
+        <v>567.3080101575117</v>
       </c>
       <c r="U13">
-        <v>514.0355721252932</v>
+        <v>512.3048881643047</v>
       </c>
       <c r="V13">
-        <v>493.6424332179319</v>
+        <v>492.3311778949963</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -1401,43 +1401,43 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.516500735759003</v>
+        <v>27.59809698814373</v>
       </c>
       <c r="E14">
-        <v>1.658009997523121</v>
+        <v>38.44540183260668</v>
       </c>
       <c r="F14">
-        <v>2.096724917376689</v>
+        <v>115.8589374133198</v>
       </c>
       <c r="G14">
-        <v>2.881754965632149</v>
+        <v>170.7581151357477</v>
       </c>
       <c r="H14">
-        <v>2.867229007583833</v>
+        <v>171.9046939261023</v>
       </c>
       <c r="I14">
-        <v>1.433512597090133</v>
+        <v>120.4893558152518</v>
       </c>
       <c r="J14">
-        <v>3.626687400423816</v>
+        <v>52.2628412471144</v>
       </c>
       <c r="K14">
-        <v>3.379895878061367</v>
+        <v>28.31234334638594</v>
       </c>
       <c r="L14">
-        <v>4.000447390135247</v>
+        <v>17.83900293929106</v>
       </c>
       <c r="M14">
-        <v>4.801914332256297</v>
+        <v>12.5939441407318</v>
       </c>
       <c r="N14">
-        <v>4.155567300485678</v>
+        <v>9.480095953501099</v>
       </c>
       <c r="O14">
-        <v>3.626771209981159</v>
+        <v>7.319607890530854</v>
       </c>
       <c r="P14">
-        <v>3.192682994078432</v>
+        <v>5.738900787893129</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1463,64 +1463,64 @@
         <v>34</v>
       </c>
       <c r="C15">
-        <v>64.69058476983885</v>
+        <v>85.90638682504824</v>
       </c>
       <c r="D15">
-        <v>159.4777139936874</v>
+        <v>227.1193857113478</v>
       </c>
       <c r="E15">
-        <v>195.8528362154138</v>
+        <v>373.7320552553804</v>
       </c>
       <c r="F15">
-        <v>234.0483214083228</v>
+        <v>494.5660569401317</v>
       </c>
       <c r="G15">
-        <v>306.3844753316204</v>
+        <v>543.996178510354</v>
       </c>
       <c r="H15">
-        <v>309.052890637555</v>
+        <v>549.7010761661747</v>
       </c>
       <c r="I15">
-        <v>290.6372606387285</v>
+        <v>566.2230104844134</v>
       </c>
       <c r="J15">
-        <v>345.6558753285826</v>
+        <v>572.0039704097823</v>
       </c>
       <c r="K15">
-        <v>303.0282199768795</v>
+        <v>503.558802977895</v>
       </c>
       <c r="L15">
-        <v>314.8075771120157</v>
+        <v>477.9819149723425</v>
       </c>
       <c r="M15">
-        <v>312.0138358054693</v>
+        <v>399.0928196254592</v>
       </c>
       <c r="N15">
-        <v>216.9290024465496</v>
+        <v>351.1706055039873</v>
       </c>
       <c r="O15">
-        <v>140.4700853451954</v>
+        <v>294.9754909567114</v>
       </c>
       <c r="P15">
-        <v>99.17538785329646</v>
+        <v>179.8881236575081</v>
       </c>
       <c r="Q15">
-        <v>76.30344540203792</v>
+        <v>119.2426325526921</v>
       </c>
       <c r="R15">
-        <v>52.80589530857267</v>
+        <v>87.99178959921917</v>
       </c>
       <c r="S15">
-        <v>34.26957718444832</v>
+        <v>57.76534203168423</v>
       </c>
       <c r="T15">
-        <v>21.0562012630411</v>
+        <v>33.77334677282705</v>
       </c>
       <c r="U15">
-        <v>17.0393003371521</v>
+        <v>27.37792906988312</v>
       </c>
       <c r="V15">
-        <v>13.15229110538708</v>
+        <v>19.39159139457361</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -1528,64 +1528,64 @@
         <v>35</v>
       </c>
       <c r="C16">
-        <v>140.4776559578056</v>
+        <v>159.8572755789777</v>
       </c>
       <c r="D16">
-        <v>305.7659590513069</v>
+        <v>366.0927270761897</v>
       </c>
       <c r="E16">
-        <v>587.424799267814</v>
+        <v>647.8255545715936</v>
       </c>
       <c r="F16">
-        <v>774.5267960136396</v>
+        <v>846.2642408997592</v>
       </c>
       <c r="G16">
-        <v>869.3458722846331</v>
+        <v>1015.839400631653</v>
       </c>
       <c r="H16">
-        <v>887.1577571207788</v>
+        <v>960.6326498654468</v>
       </c>
       <c r="I16">
-        <v>939.55262651209</v>
+        <v>1016.517476684082</v>
       </c>
       <c r="J16">
-        <v>931.9165842184208</v>
+        <v>1042.997736992703</v>
       </c>
       <c r="K16">
-        <v>819.3278879907612</v>
+        <v>878.6541889429345</v>
       </c>
       <c r="L16">
-        <v>710.7327741828678</v>
+        <v>794.3873163155865</v>
       </c>
       <c r="M16">
-        <v>540.3181330518578</v>
+        <v>697.1994894555528</v>
       </c>
       <c r="N16">
-        <v>478.8819839644657</v>
+        <v>628.00272350457</v>
       </c>
       <c r="O16">
-        <v>398.3789228402492</v>
+        <v>482.8170123692468</v>
       </c>
       <c r="P16">
-        <v>271.5969842102515</v>
+        <v>329.1129699311181</v>
       </c>
       <c r="Q16">
-        <v>171.0632474691374</v>
+        <v>236.9597079275382</v>
       </c>
       <c r="R16">
-        <v>112.735493698308</v>
+        <v>154.5452599192011</v>
       </c>
       <c r="S16">
-        <v>81.30320933800061</v>
+        <v>97.98141751806412</v>
       </c>
       <c r="T16">
-        <v>65.9657193274747</v>
+        <v>74.20063645099799</v>
       </c>
       <c r="U16">
-        <v>55.10559753811332</v>
+        <v>59.80625715607492</v>
       </c>
       <c r="V16">
-        <v>37.40232405807912</v>
+        <v>44.418565214639</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -1593,64 +1593,64 @@
         <v>36</v>
       </c>
       <c r="C17">
-        <v>344.5617067866932</v>
+        <v>395.8606201310957</v>
       </c>
       <c r="D17">
-        <v>795.5610449543606</v>
+        <v>800.9595667066051</v>
       </c>
       <c r="E17">
-        <v>1106.359693582789</v>
+        <v>1352.128990207339</v>
       </c>
       <c r="F17">
-        <v>1178.834878459242</v>
+        <v>1411.269489330544</v>
       </c>
       <c r="G17">
-        <v>1328.596150125175</v>
+        <v>1581.498611352788</v>
       </c>
       <c r="H17">
-        <v>1590.667605088753</v>
+        <v>1749.427215352035</v>
       </c>
       <c r="I17">
-        <v>1622.272513580028</v>
+        <v>1719.215028938294</v>
       </c>
       <c r="J17">
-        <v>1728.388539730485</v>
+        <v>1762.149222984638</v>
       </c>
       <c r="K17">
-        <v>1610.479785024642</v>
+        <v>1699.695271884009</v>
       </c>
       <c r="L17">
-        <v>1499.875894650472</v>
+        <v>1528.594207132125</v>
       </c>
       <c r="M17">
-        <v>1316.713771335951</v>
+        <v>1506.14316467869</v>
       </c>
       <c r="N17">
-        <v>1228.464941091664</v>
+        <v>1425.565531213652</v>
       </c>
       <c r="O17">
-        <v>999.0556349567561</v>
+        <v>1091.828647768122</v>
       </c>
       <c r="P17">
-        <v>858.2440324472431</v>
+        <v>902.8259448621068</v>
       </c>
       <c r="Q17">
-        <v>749.7961923103936</v>
+        <v>774.9854024249636</v>
       </c>
       <c r="R17">
-        <v>468.9206353528774</v>
+        <v>511.5157358433776</v>
       </c>
       <c r="S17">
-        <v>299.3752913978469</v>
+        <v>320.632028957194</v>
       </c>
       <c r="T17">
-        <v>224.5746068764272</v>
+        <v>231.8351086712019</v>
       </c>
       <c r="U17">
-        <v>124.5847986757773</v>
+        <v>133.274865301005</v>
       </c>
       <c r="V17">
-        <v>109.1715294584409</v>
+        <v>115.3676212829785</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -1658,64 +1658,64 @@
         <v>37</v>
       </c>
       <c r="C18">
-        <v>3858.281431215651</v>
+        <v>3858.284906931097</v>
       </c>
       <c r="D18">
-        <v>5006.318502195393</v>
+        <v>5006.321567132402</v>
       </c>
       <c r="E18">
         <v>6620.195513697532</v>
       </c>
       <c r="F18">
-        <v>6781.409826678473</v>
+        <v>6781.410831816548</v>
       </c>
       <c r="G18">
-        <v>8968.133032954333</v>
+        <v>8968.132758815722</v>
       </c>
       <c r="H18">
-        <v>10248.82631385416</v>
+        <v>10248.82600825178</v>
       </c>
       <c r="I18">
-        <v>10443.23211779421</v>
+        <v>10443.2322406751</v>
       </c>
       <c r="J18">
-        <v>10183.05212786518</v>
+        <v>10183.05233112912</v>
       </c>
       <c r="K18">
-        <v>9681.84895782672</v>
+        <v>9681.848999987094</v>
       </c>
       <c r="L18">
-        <v>9263.33648290893</v>
+        <v>9263.336642351107</v>
       </c>
       <c r="M18">
-        <v>8600.148761154667</v>
+        <v>8600.148870937361</v>
       </c>
       <c r="N18">
-        <v>7878.668704203131</v>
+        <v>7878.668823843964</v>
       </c>
       <c r="O18">
-        <v>7043.482398893068</v>
+        <v>7043.482425699912</v>
       </c>
       <c r="P18">
-        <v>6372.053987414881</v>
+        <v>6372.054079267165</v>
       </c>
       <c r="Q18">
-        <v>5231.540730670487</v>
+        <v>5231.540780688945</v>
       </c>
       <c r="R18">
-        <v>4147.629781810328</v>
+        <v>4147.629694390414</v>
       </c>
       <c r="S18">
-        <v>4406.245289672</v>
+        <v>4406.245349718633</v>
       </c>
       <c r="T18">
-        <v>4131.941208744907</v>
+        <v>4131.941378170714</v>
       </c>
       <c r="U18">
-        <v>3849.479355905137</v>
+        <v>3849.479391138518</v>
       </c>
       <c r="V18">
-        <v>3599.268303743567</v>
+        <v>3599.26841923676</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -1723,64 +1723,64 @@
         <v>38</v>
       </c>
       <c r="C19">
-        <v>24711.27212191505</v>
+        <v>26302.90820296513</v>
       </c>
       <c r="D19">
-        <v>47663.02190398324</v>
+        <v>51549.76493914476</v>
       </c>
       <c r="E19">
-        <v>65892.48469001337</v>
+        <v>71526.62991844272</v>
       </c>
       <c r="F19">
-        <v>77331.5852486917</v>
+        <v>84456.49077045888</v>
       </c>
       <c r="G19">
-        <v>86844.79610227011</v>
+        <v>94711.6892061158</v>
       </c>
       <c r="H19">
-        <v>90761.63518448896</v>
+        <v>99256.37399210723</v>
       </c>
       <c r="I19">
-        <v>90562.9211429244</v>
+        <v>98639.62523130715</v>
       </c>
       <c r="J19">
-        <v>87599.35399939233</v>
+        <v>95909.25761353894</v>
       </c>
       <c r="K19">
-        <v>82059.18575077536</v>
+        <v>89944.87574721324</v>
       </c>
       <c r="L19">
-        <v>75792.75370444829</v>
+        <v>82915.78517363631</v>
       </c>
       <c r="M19">
-        <v>68916.37469653413</v>
+        <v>75387.33305515998</v>
       </c>
       <c r="N19">
-        <v>61330.88591071882</v>
+        <v>66964.10113749919</v>
       </c>
       <c r="O19">
-        <v>52821.43663023481</v>
+        <v>57898.22871401697</v>
       </c>
       <c r="P19">
-        <v>43242.9756714706</v>
+        <v>47176.41292248949</v>
       </c>
       <c r="Q19">
-        <v>33240.50026465535</v>
+        <v>36164.69171778169</v>
       </c>
       <c r="R19">
-        <v>23946.27617804996</v>
+        <v>25987.80881768425</v>
       </c>
       <c r="S19">
-        <v>17732.36377859286</v>
+        <v>18979.73999320466</v>
       </c>
       <c r="T19">
-        <v>13316.64174913288</v>
+        <v>14091.88997808917</v>
       </c>
       <c r="U19">
-        <v>9537.296897823808</v>
+        <v>10065.79821651878</v>
       </c>
       <c r="V19">
-        <v>7777.001857412648</v>
+        <v>8163.278163619487</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -1851,19 +1851,19 @@
         <v>28</v>
       </c>
       <c r="W20">
-        <v>465611.8760978373</v>
+        <v>473846.1710069214</v>
       </c>
       <c r="X20">
-        <v>171122.5724094793</v>
+        <v>171776.7885033703</v>
       </c>
       <c r="Y20">
-        <v>109464.2683831134</v>
+        <v>110783.9191902349</v>
       </c>
       <c r="Z20">
-        <v>855843.0401010838</v>
+        <v>866778.165361596</v>
       </c>
       <c r="AA20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -1871,64 +1871,64 @@
         <v>31</v>
       </c>
       <c r="C21">
-        <v>443.6782466537567</v>
+        <v>448.0019393849169</v>
       </c>
       <c r="D21">
-        <v>963.4040348920937</v>
+        <v>976.7122977459101</v>
       </c>
       <c r="E21">
-        <v>1403.295772232517</v>
+        <v>1438.787993790288</v>
       </c>
       <c r="F21">
-        <v>1796.366655542664</v>
+        <v>1834.051234891751</v>
       </c>
       <c r="G21">
-        <v>2034.409428185783</v>
+        <v>2072.813233907636</v>
       </c>
       <c r="H21">
-        <v>2154.041017788792</v>
+        <v>2215.584681238321</v>
       </c>
       <c r="I21">
-        <v>2228.426178811914</v>
+        <v>2280.832661688695</v>
       </c>
       <c r="J21">
-        <v>2256.160831533132</v>
+        <v>2278.100978721813</v>
       </c>
       <c r="K21">
-        <v>2240.613704287256</v>
+        <v>2249.987345528053</v>
       </c>
       <c r="L21">
-        <v>2173.762633521106</v>
+        <v>2191.658775004028</v>
       </c>
       <c r="M21">
-        <v>2064.278847389741</v>
+        <v>2074.351075236801</v>
       </c>
       <c r="N21">
-        <v>1922.685689682292</v>
+        <v>1924.84914891905</v>
       </c>
       <c r="O21">
-        <v>1717.121209910609</v>
+        <v>1726.692725956492</v>
       </c>
       <c r="P21">
-        <v>1481.048140167356</v>
+        <v>1487.384113698283</v>
       </c>
       <c r="Q21">
-        <v>1158.204676784645</v>
+        <v>1163.757590716563</v>
       </c>
       <c r="R21">
-        <v>843.2250397470667</v>
+        <v>855.5701928484675</v>
       </c>
       <c r="S21">
-        <v>593.7137173124626</v>
+        <v>604.2835224615476</v>
       </c>
       <c r="T21">
-        <v>456.7265910883791</v>
+        <v>463.8183976892191</v>
       </c>
       <c r="U21">
-        <v>370.5538684944836</v>
+        <v>369.5189576367937</v>
       </c>
       <c r="V21">
-        <v>255.7894803141722</v>
+        <v>265.8920824033536</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -1936,64 +1936,64 @@
         <v>32</v>
       </c>
       <c r="C22">
-        <v>361.8593783139974</v>
+        <v>347.5874861368498</v>
       </c>
       <c r="D22">
-        <v>842.5788001356258</v>
+        <v>817.5120894069104</v>
       </c>
       <c r="E22">
-        <v>1144.242830599349</v>
+        <v>1093.637988108999</v>
       </c>
       <c r="F22">
-        <v>1539.125103079044</v>
+        <v>1466.956298628701</v>
       </c>
       <c r="G22">
-        <v>1827.834100552929</v>
+        <v>1756.061221956732</v>
       </c>
       <c r="H22">
-        <v>2039.422408731447</v>
+        <v>1968.28666545187</v>
       </c>
       <c r="I22">
-        <v>2122.515835051558</v>
+        <v>2045.28275033297</v>
       </c>
       <c r="J22">
-        <v>2144.308701352348</v>
+        <v>2078.475300058232</v>
       </c>
       <c r="K22">
-        <v>2160.802085604077</v>
+        <v>2098.907468895638</v>
       </c>
       <c r="L22">
-        <v>2129.658387119248</v>
+        <v>2070.075231799045</v>
       </c>
       <c r="M22">
-        <v>2035.789205885535</v>
+        <v>1987.372555186791</v>
       </c>
       <c r="N22">
-        <v>1917.16266455663</v>
+        <v>1880.753206583665</v>
       </c>
       <c r="O22">
-        <v>1789.897377134378</v>
+        <v>1762.634116370083</v>
       </c>
       <c r="P22">
-        <v>1588.653047633204</v>
+        <v>1570.120516138032</v>
       </c>
       <c r="Q22">
-        <v>1185.007462179203</v>
+        <v>1171.249963860291</v>
       </c>
       <c r="R22">
-        <v>822.0209739272974</v>
+        <v>816.3388724854406</v>
       </c>
       <c r="S22">
-        <v>582.6115198361816</v>
+        <v>578.6869258497233</v>
       </c>
       <c r="T22">
-        <v>493.9071458889419</v>
+        <v>485.961328267521</v>
       </c>
       <c r="U22">
-        <v>434.435501540875</v>
+        <v>411.3367531456702</v>
       </c>
       <c r="V22">
-        <v>350.9576822924346</v>
+        <v>350.2091159624409</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -2001,64 +2001,64 @@
         <v>33</v>
       </c>
       <c r="C23">
-        <v>1.543776635232449</v>
+        <v>51.8692304945022</v>
       </c>
       <c r="D23">
-        <v>6.098182868164356</v>
+        <v>145.1374375397223</v>
       </c>
       <c r="E23">
-        <v>11.47129448140096</v>
+        <v>213.4886468887786</v>
       </c>
       <c r="F23">
-        <v>15.76880970526454</v>
+        <v>213.9162406469565</v>
       </c>
       <c r="G23">
-        <v>19.02084793976713</v>
+        <v>230.6059707386206</v>
       </c>
       <c r="H23">
-        <v>22.02549472502801</v>
+        <v>254.3657529655084</v>
       </c>
       <c r="I23">
-        <v>24.49501464097899</v>
+        <v>239.5537367849938</v>
       </c>
       <c r="J23">
-        <v>28.09771384587408</v>
+        <v>219.7948689056078</v>
       </c>
       <c r="K23">
-        <v>35.21103499027677</v>
+        <v>203.0610865853044</v>
       </c>
       <c r="L23">
-        <v>40.41076915772037</v>
+        <v>185.0796117664435</v>
       </c>
       <c r="M23">
-        <v>39.95997679272215</v>
+        <v>168.8964308788411</v>
       </c>
       <c r="N23">
-        <v>38.47586163728279</v>
+        <v>154.3075532438415</v>
       </c>
       <c r="O23">
-        <v>36.14819635071219</v>
+        <v>141.4984118167566</v>
       </c>
       <c r="P23">
-        <v>32.87663894161927</v>
+        <v>116.2574780633695</v>
       </c>
       <c r="Q23">
-        <v>28.93984874645751</v>
+        <v>98.20528779575854</v>
       </c>
       <c r="R23">
-        <v>25.00955595369539</v>
+        <v>82.1793816445167</v>
       </c>
       <c r="S23">
-        <v>20.91639807280468</v>
+        <v>58.05251088466392</v>
       </c>
       <c r="T23">
-        <v>16.46834139790871</v>
+        <v>42.24292656399084</v>
       </c>
       <c r="U23">
-        <v>12.40360373688751</v>
+        <v>22.4705656994188</v>
       </c>
       <c r="V23">
-        <v>8.447431347002322</v>
+        <v>16.81619315100032</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -2066,64 +2066,64 @@
         <v>34</v>
       </c>
       <c r="C24">
-        <v>244.6657013817266</v>
+        <v>229.2819745620249</v>
       </c>
       <c r="D24">
-        <v>406.4333407840412</v>
+        <v>503.6955066054448</v>
       </c>
       <c r="E24">
-        <v>533.4672758105194</v>
+        <v>757.413688651038</v>
       </c>
       <c r="F24">
-        <v>613.4023410485831</v>
+        <v>795.5555153257396</v>
       </c>
       <c r="G24">
-        <v>638.0695373800486</v>
+        <v>853.851344418949</v>
       </c>
       <c r="H24">
-        <v>687.6648671412538</v>
+        <v>826.4884385750563</v>
       </c>
       <c r="I24">
-        <v>703.1312009899962</v>
+        <v>832.8457361664721</v>
       </c>
       <c r="J24">
-        <v>683.8233882446706</v>
+        <v>804.8028438283757</v>
       </c>
       <c r="K24">
-        <v>659.5811473128397</v>
+        <v>815.3925311935861</v>
       </c>
       <c r="L24">
-        <v>619.2746953574311</v>
+        <v>796.8473376828169</v>
       </c>
       <c r="M24">
-        <v>584.1245227771234</v>
+        <v>724.0114458408051</v>
       </c>
       <c r="N24">
-        <v>598.6905332389799</v>
+        <v>639.70175044332</v>
       </c>
       <c r="O24">
-        <v>520.2053483763409</v>
+        <v>550.8718315491955</v>
       </c>
       <c r="P24">
-        <v>420.6869969260913</v>
+        <v>460.182443512971</v>
       </c>
       <c r="Q24">
-        <v>365.7916991219701</v>
+        <v>361.1716523147335</v>
       </c>
       <c r="R24">
-        <v>311.6856180795157</v>
+        <v>298.5036435743702</v>
       </c>
       <c r="S24">
-        <v>242.0920397422883</v>
+        <v>227.8290077597616</v>
       </c>
       <c r="T24">
-        <v>157.7169928608645</v>
+        <v>156.9796118437802</v>
       </c>
       <c r="U24">
-        <v>118.1277399221664</v>
+        <v>118.1279175438766</v>
       </c>
       <c r="V24">
-        <v>92.8393481851615</v>
+        <v>92.83952972172315</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -2131,64 +2131,64 @@
         <v>35</v>
       </c>
       <c r="C25">
-        <v>374.4965971710429</v>
+        <v>362.7314222518877</v>
       </c>
       <c r="D25">
-        <v>762.9746132316765</v>
+        <v>762.973060571727</v>
       </c>
       <c r="E25">
-        <v>1060.203549767089</v>
+        <v>1056.893060977454</v>
       </c>
       <c r="F25">
-        <v>1234.800189667622</v>
+        <v>1267.762493022714</v>
       </c>
       <c r="G25">
-        <v>1480.300612237588</v>
+        <v>1572.396578887442</v>
       </c>
       <c r="H25">
-        <v>1561.335300548603</v>
+        <v>1698.69149246993</v>
       </c>
       <c r="I25">
-        <v>1548.030087695231</v>
+        <v>1817.397224930503</v>
       </c>
       <c r="J25">
-        <v>1528.346981632666</v>
+        <v>1798.352417057966</v>
       </c>
       <c r="K25">
-        <v>1464.752803539686</v>
+        <v>1694.987220792171</v>
       </c>
       <c r="L25">
-        <v>1377.12032729975</v>
+        <v>1538.511638296976</v>
       </c>
       <c r="M25">
-        <v>1336.094682961306</v>
+        <v>1400.351834827014</v>
       </c>
       <c r="N25">
-        <v>1325.547345803753</v>
+        <v>1235.968312793155</v>
       </c>
       <c r="O25">
-        <v>1025.236822726421</v>
+        <v>1086.513252127157</v>
       </c>
       <c r="P25">
-        <v>836.055803179779</v>
+        <v>895.883759309913</v>
       </c>
       <c r="Q25">
-        <v>594.861896680884</v>
+        <v>672.1801056446313</v>
       </c>
       <c r="R25">
-        <v>425.167031451211</v>
+        <v>466.4174348370232</v>
       </c>
       <c r="S25">
-        <v>315.2435486826237</v>
+        <v>312.7283251697268</v>
       </c>
       <c r="T25">
-        <v>236.4514261963303</v>
+        <v>233.9080349804838</v>
       </c>
       <c r="U25">
-        <v>174.0692035722401</v>
+        <v>174.0689894272341</v>
       </c>
       <c r="V25">
-        <v>124.6895596458588</v>
+        <v>124.6895474335416</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -2196,64 +2196,64 @@
         <v>36</v>
       </c>
       <c r="C26">
-        <v>569.2026261743663</v>
+        <v>571.1463811371325</v>
       </c>
       <c r="D26">
-        <v>1212.494465866802</v>
+        <v>1212.495609173849</v>
       </c>
       <c r="E26">
-        <v>1955.628769002987</v>
+        <v>1955.628051106579</v>
       </c>
       <c r="F26">
-        <v>2434.694117260341</v>
+        <v>2434.693356500207</v>
       </c>
       <c r="G26">
-        <v>2992.917039532127</v>
+        <v>2992.917989706055</v>
       </c>
       <c r="H26">
-        <v>3588.837971087195</v>
+        <v>3376.134087018368</v>
       </c>
       <c r="I26">
-        <v>3865.652128032961</v>
+        <v>3444.842085134264</v>
       </c>
       <c r="J26">
-        <v>3784.556337159815</v>
+        <v>3436.59342862657</v>
       </c>
       <c r="K26">
-        <v>3613.377939052695</v>
+        <v>3268.767201247054</v>
       </c>
       <c r="L26">
-        <v>3351.150613346988</v>
+        <v>3090.521858851377</v>
       </c>
       <c r="M26">
-        <v>3085.81703889543</v>
+        <v>3012.788980121206</v>
       </c>
       <c r="N26">
-        <v>3033.532933264051</v>
+        <v>2957.405967305655</v>
       </c>
       <c r="O26">
-        <v>2569.496099975859</v>
+        <v>2545.500054524631</v>
       </c>
       <c r="P26">
-        <v>2161.912156102348</v>
+        <v>2163.693326482557</v>
       </c>
       <c r="Q26">
-        <v>1769.758482945159</v>
+        <v>1801.190571061411</v>
       </c>
       <c r="R26">
-        <v>1271.159076036672</v>
+        <v>1367.653252124958</v>
       </c>
       <c r="S26">
-        <v>903.8000710384445</v>
+        <v>903.8006646100364</v>
       </c>
       <c r="T26">
-        <v>535.84519718857</v>
+        <v>604.217759333404</v>
       </c>
       <c r="U26">
-        <v>461.7807260492227</v>
+        <v>476.9376127876237</v>
       </c>
       <c r="V26">
-        <v>208.8441352773053</v>
+        <v>230.8698640023696</v>
       </c>
     </row>
     <row r="27" spans="1:27">
@@ -2261,7 +2261,7 @@
         <v>37</v>
       </c>
       <c r="C27">
-        <v>1665.004031474981</v>
+        <v>1599.071198557182</v>
       </c>
       <c r="D27">
         <v>3960.838731569926</v>
@@ -2276,49 +2276,49 @@
         <v>7437.037959901335</v>
       </c>
       <c r="H27">
-        <v>9046.439105621774</v>
+        <v>9046.437959817722</v>
       </c>
       <c r="I27">
-        <v>9566.796892411188</v>
+        <v>9566.794580204833</v>
       </c>
       <c r="J27">
-        <v>9843.048325125856</v>
+        <v>9843.046279068405</v>
       </c>
       <c r="K27">
-        <v>10043.91290342726</v>
+        <v>10043.91171350932</v>
       </c>
       <c r="L27">
-        <v>9954.173837864944</v>
+        <v>9954.173921107971</v>
       </c>
       <c r="M27">
-        <v>9621.855013641352</v>
+        <v>9621.855311878877</v>
       </c>
       <c r="N27">
-        <v>9133.675257549938</v>
+        <v>9133.674309114305</v>
       </c>
       <c r="O27">
-        <v>8570.98680761433</v>
+        <v>8570.985889542053</v>
       </c>
       <c r="P27">
-        <v>7636.955613259365</v>
+        <v>7636.954855722198</v>
       </c>
       <c r="Q27">
-        <v>5368.939801829926</v>
+        <v>5368.939138667408</v>
       </c>
       <c r="R27">
-        <v>3441.016532458541</v>
+        <v>3441.015730005971</v>
       </c>
       <c r="S27">
-        <v>2273.396187806227</v>
+        <v>2273.396324869156</v>
       </c>
       <c r="T27">
-        <v>1667.11969137785</v>
+        <v>1667.119173128749</v>
       </c>
       <c r="U27">
-        <v>1644.246086897411</v>
+        <v>1644.24656931661</v>
       </c>
       <c r="V27">
-        <v>1564.540086236301</v>
+        <v>1564.540044008472</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -2326,64 +2326,64 @@
         <v>38</v>
       </c>
       <c r="C28">
-        <v>13310.3473996127</v>
+        <v>13440.05818154751</v>
       </c>
       <c r="D28">
-        <v>28902.12104676282</v>
+        <v>29301.3689323773</v>
       </c>
       <c r="E28">
-        <v>42098.87316697551</v>
+        <v>43163.63981370863</v>
       </c>
       <c r="F28">
-        <v>53890.99966627994</v>
+        <v>55021.53704675251</v>
       </c>
       <c r="G28">
-        <v>61032.28284557348</v>
+        <v>62184.39701722906</v>
       </c>
       <c r="H28">
-        <v>64621.23053366376</v>
+        <v>66467.54043714963</v>
       </c>
       <c r="I28">
-        <v>66852.78536435745</v>
+        <v>68424.97985066086</v>
       </c>
       <c r="J28">
-        <v>67684.82494599397</v>
+        <v>68343.02936165439</v>
       </c>
       <c r="K28">
-        <v>67218.41112861766</v>
+        <v>67499.62036584156</v>
       </c>
       <c r="L28">
-        <v>65212.87900563317</v>
+        <v>65749.76325012084</v>
       </c>
       <c r="M28">
-        <v>61928.36542169224</v>
+        <v>62230.53225710402</v>
       </c>
       <c r="N28">
-        <v>57680.57069046876</v>
+        <v>57745.4744675715</v>
       </c>
       <c r="O28">
-        <v>51513.63629731828</v>
+        <v>51800.78177869476</v>
       </c>
       <c r="P28">
-        <v>44431.44420502068</v>
+        <v>44621.5234109485</v>
       </c>
       <c r="Q28">
-        <v>34746.14030353935</v>
+        <v>34912.72772149691</v>
       </c>
       <c r="R28">
-        <v>25296.751192412</v>
+        <v>25667.10578545402</v>
       </c>
       <c r="S28">
-        <v>17811.41151937387</v>
+        <v>18128.50567384643</v>
       </c>
       <c r="T28">
-        <v>13701.79773265137</v>
+        <v>13914.55193067657</v>
       </c>
       <c r="U28">
-        <v>10746.06218634002</v>
+        <v>10716.04977146701</v>
       </c>
       <c r="V28">
-        <v>7162.105448796823</v>
+        <v>7444.978307293903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>